<commit_message>
Worked on Q breakdown
</commit_message>
<xml_diff>
--- a/projects/AAR_final-project/Questionnaire Breakdown.xlsx
+++ b/projects/AAR_final-project/Questionnaire Breakdown.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="113">
   <si>
     <t>Q Num</t>
   </si>
@@ -229,6 +229,132 @@
   </si>
   <si>
     <t>Have a VR device at A1</t>
+  </si>
+  <si>
+    <t>Overall consumption</t>
+  </si>
+  <si>
+    <t>B1:1</t>
+  </si>
+  <si>
+    <t>B1:2</t>
+  </si>
+  <si>
+    <t>B1:3</t>
+  </si>
+  <si>
+    <t>B1:4</t>
+  </si>
+  <si>
+    <t>B1:5</t>
+  </si>
+  <si>
+    <t>B1:6</t>
+  </si>
+  <si>
+    <t>B1:7</t>
+  </si>
+  <si>
+    <t>B1:8</t>
+  </si>
+  <si>
+    <t>B1:9</t>
+  </si>
+  <si>
+    <t>B1:10</t>
+  </si>
+  <si>
+    <t>B1:11</t>
+  </si>
+  <si>
+    <t>B1a: 1</t>
+  </si>
+  <si>
+    <t>B1a: 2</t>
+  </si>
+  <si>
+    <t>B1a: 3</t>
+  </si>
+  <si>
+    <t>B1a: 4</t>
+  </si>
+  <si>
+    <t>B1a: 5</t>
+  </si>
+  <si>
+    <t>B1a: 6</t>
+  </si>
+  <si>
+    <t>B1a: 7</t>
+  </si>
+  <si>
+    <t>B1a: 8</t>
+  </si>
+  <si>
+    <t>B1a: 9</t>
+  </si>
+  <si>
+    <t>1+ at corresponding B1 Q</t>
+  </si>
+  <si>
+    <t>TV:Buy: Full Season: DVD (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV:Buy: Full Season: Blu-ray (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV:Buy: Full Season: Digital (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV:Buy: Episode: Digital (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV: Rent: Full Season: Disc: Walk-in (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV: Rent: Full Season: Disc: Mail (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV: Rent: Full Season: Digital: Sub Stream (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV: Rent: Episode: Digital: Sub Stream (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV: Free: Full Season: Digital: Ad Stream (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV: Free: Episode: Digital: Ad Stream (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV: Free: Episode: Digital: cVOD (# P6M: Total)</t>
+  </si>
+  <si>
+    <t>TV:Buy: Full Season: DVD (# P6M: Fam)</t>
+  </si>
+  <si>
+    <t>TV:Buy: Full Season: Blu-ray (# P6M: Fam)</t>
+  </si>
+  <si>
+    <t>TV:Buy: Full Season: Digital (# P6M: Fam)</t>
+  </si>
+  <si>
+    <t>TV:Buy: Episode: Digital (# P6M: Fam)</t>
+  </si>
+  <si>
+    <t>TV: Rent: Full Season: Disc: Walk-in (# P6M: Fam)</t>
+  </si>
+  <si>
+    <t>TV: Rent: Full Season: Disc: Mail (# P6M: Fam)</t>
+  </si>
+  <si>
+    <t>TV: Rent: Full Season: Digital: Sub Stream (# P6M: Fam)</t>
+  </si>
+  <si>
+    <t>TV: Rent: Episode: Digital: Sub Stream (# P6M: Fam)</t>
+  </si>
+  <si>
+    <t>TV: Free: Full Season: Digital: Ad Stream (# P6M: Fam)</t>
   </si>
 </sst>
 </file>
@@ -609,17 +735,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="2" max="2" width="19.08984375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="51.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -1123,113 +1250,380 @@
       <c r="A26" s="3">
         <v>25</v>
       </c>
+      <c r="B26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
+      <c r="B27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
+      <c r="B28" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
+      <c r="B29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
+      <c r="B30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
+      <c r="B31" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B32" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B33" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B35" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B37" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B38" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B39" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" t="s">
+        <v>106</v>
+      </c>
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B41" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" t="s">
+        <v>109</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B43" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B44" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B45" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" t="s">
+        <v>112</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -1336,8 +1730,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>